<commit_message>
Kansas water rights update
Kansas water rights update
</commit_message>
<xml_diff>
--- a/Kansas/WaterAllocation/KS_Allocation Schema Mapping to WaDE_QA.xlsx
+++ b/Kansas/WaterAllocation/KS_Allocation Schema Mapping to WaDE_QA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjame\Documents\WSWC Documents\MappingStatesDataToWaDE2.0\Kansas\WaterAllocation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA1CF70-1BAE-4656-944F-E3E46C518E55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80544103-76F0-4BD6-A7B7-2ECF87A0CD88}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="714" activeTab="8" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="714" activeTab="6" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping Notes" sheetId="10" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1577" uniqueCount="826">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1584" uniqueCount="829">
   <si>
     <t>Name</t>
   </si>
@@ -2563,6 +2563,15 @@
   </si>
   <si>
     <t>Proposed Certificate Extended Time to Perfect</t>
+  </si>
+  <si>
+    <t>OwnerClassificationCV</t>
+  </si>
+  <si>
+    <t>Army (USA)</t>
+  </si>
+  <si>
+    <t>WSWC defined owner tag.</t>
   </si>
 </sst>
 </file>
@@ -3353,7 +3362,7 @@
     <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3640,6 +3649,9 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="23" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -6313,10 +6325,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B91B1FF-D207-4871-B787-27544A9D3030}">
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46:G46"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43:XFD43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7297,7 +7309,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>101</v>
       </c>
@@ -7329,7 +7341,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>98</v>
       </c>
@@ -7361,7 +7373,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="35" spans="1:10" s="51" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" s="51" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>100</v>
       </c>
@@ -7393,7 +7405,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" s="51" t="s">
         <v>154</v>
       </c>
@@ -7421,7 +7433,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>82</v>
       </c>
@@ -7453,7 +7465,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="38" spans="1:10" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" s="51" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="92" t="s">
         <v>808</v>
       </c>
@@ -7479,7 +7491,7 @@
       <c r="I38" s="97"/>
       <c r="J38" s="98"/>
     </row>
-    <row r="39" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>90</v>
       </c>
@@ -7511,7 +7523,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>91</v>
       </c>
@@ -7541,7 +7553,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>99</v>
       </c>
@@ -7573,7 +7585,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>96</v>
       </c>
@@ -7605,50 +7617,50 @@
         <v>159</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16" s="51" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>89</v>
+        <v>826</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D43" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E43" s="25" t="s">
-        <v>569</v>
-      </c>
-      <c r="F43" s="35" t="s">
-        <v>38</v>
-      </c>
-      <c r="G43" s="48" t="s">
-        <v>38</v>
-      </c>
+      <c r="D43" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="101"/>
       <c r="H43" s="39" t="s">
         <v>38</v>
       </c>
       <c r="I43" s="66" t="s">
-        <v>38</v>
+        <v>827</v>
       </c>
       <c r="J43" s="62" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" s="51" customFormat="1" x14ac:dyDescent="0.3">
+        <v>828</v>
+      </c>
+      <c r="K43" s="5"/>
+      <c r="L43" s="5"/>
+      <c r="M43" s="5"/>
+      <c r="N43" s="5"/>
+      <c r="O43" s="5"/>
+      <c r="P43" s="5"/>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="C44" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="E44" s="25" t="s">
         <v>569</v>
@@ -7662,80 +7674,112 @@
       <c r="H44" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="I44" s="18" t="s">
+      <c r="I44" s="66" t="s">
+        <v>38</v>
+      </c>
+      <c r="J44" s="62" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E45" s="25" t="s">
+        <v>569</v>
+      </c>
+      <c r="F45" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="G45" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="H45" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="I45" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="J44" s="63" t="s">
+      <c r="J45" s="63" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A45" s="51" t="s">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A46" s="51" t="s">
         <v>148</v>
       </c>
-      <c r="B45" s="52" t="s">
+      <c r="B46" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="C45" s="53" t="s">
+      <c r="C46" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="D45" s="55" t="s">
+      <c r="D46" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="E45" s="25" t="s">
+      <c r="E46" s="25" t="s">
         <v>131</v>
       </c>
-      <c r="F45" s="35" t="s">
-        <v>38</v>
-      </c>
-      <c r="G45" s="48" t="s">
-        <v>38</v>
-      </c>
-      <c r="H45" s="39" t="s">
-        <v>38</v>
-      </c>
-      <c r="I45" s="64" t="s">
+      <c r="F46" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="G46" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="H46" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="I46" s="64" t="s">
         <v>131</v>
       </c>
-      <c r="J45" s="62" t="s">
+      <c r="J46" s="62" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A46" s="5" t="s">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A47" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="B47" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="C47" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D46" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E46" s="25" t="s">
+      <c r="D47" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E47" s="25" t="s">
         <v>569</v>
       </c>
-      <c r="F46" s="35" t="s">
-        <v>38</v>
-      </c>
-      <c r="G46" s="48" t="s">
-        <v>38</v>
-      </c>
-      <c r="H46" s="39" t="s">
-        <v>38</v>
-      </c>
-      <c r="I46" s="18" t="s">
+      <c r="F47" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="G47" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="H47" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="I47" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="J46" s="62" t="s">
+      <c r="J47" s="62" t="s">
         <v>210</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A14:J45">
-    <sortCondition ref="A14:A45"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A14:J46">
+    <sortCondition ref="A14:A46"/>
   </sortState>
   <phoneticPr fontId="25" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7790,7 +7834,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4937A746-C61C-4B77-856B-5C115168800E}">
   <dimension ref="A1:D507"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="G64" sqref="G64"/>
     </sheetView>
   </sheetViews>

</xml_diff>